<commit_message>
se actualizo el excel grupos_clientes.xlsx con los nuevos nombre de grupo e integrantes de cada grupo cabio
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>NOMBRE_GRUPO</t>
   </si>
@@ -27,10 +27,55 @@
     <t>CLIENTES</t>
   </si>
   <si>
-    <t>GRUPO_SINPAR</t>
-  </si>
-  <si>
-    <t>GRUPO_MAYORISTAS</t>
+    <t>MEJORAR</t>
+  </si>
+  <si>
+    <t>233.10167.20234.20292.20357.20379.20385.50102.50818.60124.60139.60158.60174.60258.70101</t>
+  </si>
+  <si>
+    <t>PREMIUM</t>
+  </si>
+  <si>
+    <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380</t>
+  </si>
+  <si>
+    <t>PREMIUM TOP</t>
+  </si>
+  <si>
+    <t>RECURRENTE_&lt;_100K</t>
+  </si>
+  <si>
+    <t>12.20.265.938.947.970.999.1000.20094.20095.20108.20117.20140.20142.20156.20160.20169.20179.20242.20244.20249.20294.20344.20362.20364.20366</t>
+  </si>
+  <si>
+    <t>RECURRENTE_100K-200K</t>
+  </si>
+  <si>
+    <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201</t>
+  </si>
+  <si>
+    <t>RECURRENTE_200K-300K</t>
+  </si>
+  <si>
+    <t>RECURRENTE_300K-400K</t>
+  </si>
+  <si>
+    <t>RECURRENTE_400K-500K</t>
+  </si>
+  <si>
+    <t>RECURRENTE_&gt;_500K</t>
+  </si>
+  <si>
+    <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113</t>
+  </si>
+  <si>
+    <t>11.20096.20228.20238.20256.20260.20303.20361.40124.50805.60125.60191.60217.60253.61012.90504.90602.90671</t>
+  </si>
+  <si>
+    <t>939.961.962.987.1002.1010.1012.10137.10158.10162.20106.20114.20118.20137.20174.20211.20224.20230.20257.20277.20281.20289.20296.20299.20301.20306.20319.20367.20371.20372.20374.20381.20386.20388.20391.20395.50224.50812.50813.50824.50827.60128.60130.60133.60148.60163.60196.60198.60222.60257.90621</t>
+  </si>
+  <si>
+    <t>936.940.973.992.997.10163.20113.20159.20166.20173.20180.20200.20258.20272.20275.20290.20291.20331.40137.40143.50444.50607.50622.50819.50821.50825.60165.60190.60195.60202.60205.60206.60215.61004.70102.70638.90668</t>
   </si>
 </sst>
 </file>
@@ -71,10 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,17 +340,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:B994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="255.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" customWidth="1"/>
+    <col min="4" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -315,18 +366,83 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>20246.957999999999</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>950</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1301,12 +1417,6 @@
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
agregue cliente el pela cta 50815, al archivo grupo_clientes.xlsx
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -72,10 +72,10 @@
     <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425</t>
   </si>
   <si>
-    <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163</t>
-  </si>
-  <si>
     <t>233.10167.20234.20292.20357.20379.20385.50102.50818.60124.60139.60158.60174.60258.70101.3.70114</t>
+  </si>
+  <si>
+    <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163.50815</t>
   </si>
 </sst>
 </file>
@@ -342,7 +342,7 @@
   <dimension ref="A1:B994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -366,7 +366,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -374,7 +374,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
corregi errores: los precios no se mostraban en la pagina inicial, agregue ctas 90509,40144. Subi imagenes de zingueria
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -60,12 +60,6 @@
     <t>RECURRENTE_&gt;_500K</t>
   </si>
   <si>
-    <t>11.20096.20228.20238.20256.20260.20303.20361.40124.50805.60125.60191.60217.60253.61012.90504.90602.90671</t>
-  </si>
-  <si>
-    <t>939.961.962.987.1002.1010.1012.10137.10158.10162.20106.20114.20118.20137.20174.20211.20224.20230.20257.20277.20281.20289.20296.20299.20301.20306.20319.20367.20371.20372.20374.20381.20386.20388.20391.20395.50224.50812.50813.50824.50827.60128.60130.60133.60148.60163.60196.60198.60222.60257.90621</t>
-  </si>
-  <si>
     <t>936.940.973.992.997.10163.20113.20159.20166.20173.20180.20200.20258.20272.20275.20290.20291.20331.40137.40143.50444.50607.50622.50819.50821.50825.60165.60190.60195.60202.60205.60206.60215.61004.70102.70638.90668</t>
   </si>
   <si>
@@ -76,13 +70,19 @@
   </si>
   <si>
     <t>233.10167.20234.20292.20357.20379.20385.50102.50818.60124.60139.60158.60174.60258.70101.3.70114.20129</t>
+  </si>
+  <si>
+    <t>939.961.962.987.1002.1010.1012.10137.10158.10162.20106.20114.20118.20137.20174.20211.20224.20230.20257.20277.20281.20289.20296.20299.20301.20306.20319.20367.20371.20372.20374.20381.20386.20388.20391.20395.50224.50812.50813.50824.50827.60128.60130.60133.60148.60163.60196.60198.60222.60257.90621.40144</t>
+  </si>
+  <si>
+    <t>11.20096.20228.20238.20256.20260.20303.20361.40124.50805.60125.60191.60217.60253.61012.90504.90602.90671.90509</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,14 +131,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,15 +358,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="2" max="2" width="255.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.140625" customWidth="1"/>
+    <col min="3" max="3" width="114.7109375" customWidth="1"/>
     <col min="4" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -366,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -374,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -405,8 +422,8 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -414,7 +431,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -422,15 +439,15 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subi imagenes cod ISA, cod max, agreque cta 70106
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -39,9 +39,6 @@
     <t>RECURRENTE_&lt;_100K</t>
   </si>
   <si>
-    <t>12.20.265.938.947.970.999.1000.20094.20095.20108.20117.20140.20142.20156.20160.20169.20179.20242.20244.20249.20294.20344.20362.20364.20366</t>
-  </si>
-  <si>
     <t>RECURRENTE_100K-200K</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>11.20096.20228.20238.20256.20260.20303.20361.40124.50805.60125.60191.60217.60253.61012.90504.90602.90671.90509</t>
+  </si>
+  <si>
+    <t>12.20.265.938.947.970.999.1000.20094.20095.20108.20117.20140.20142.20156.20160.20169.20179.20242.20244.20249.20294.20344.20362.20364.20366.70106</t>
   </si>
 </sst>
 </file>
@@ -358,8 +358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -383,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -407,47 +407,47 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subi imagenes de codigo: px de caño
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -42,9 +42,6 @@
     <t>RECURRENTE_100K-200K</t>
   </si>
   <si>
-    <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201</t>
-  </si>
-  <si>
     <t>RECURRENTE_200K-300K</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>12.20.265.938.947.970.999.1000.20094.20095.20108.20117.20140.20142.20156.20160.20169.20179.20242.20244.20249.20294.20344.20362.20364.20366.70106</t>
+  </si>
+  <si>
+    <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201.60270.60134</t>
   </si>
 </sst>
 </file>
@@ -358,8 +358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -383,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -407,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -415,39 +415,39 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subi imagenes de polimex, igrese la cta 50808
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -60,9 +60,6 @@
     <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425</t>
   </si>
   <si>
-    <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163.50815</t>
-  </si>
-  <si>
     <t>233.10167.20234.20292.20357.20379.20385.50102.50818.60124.60139.60158.60174.60258.70101.3.70114.20129</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201.60270.60134</t>
+  </si>
+  <si>
+    <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163.50815.50808</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1:B994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -383,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -407,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -415,7 +415,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -423,7 +423,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subi imagenes de cod BA
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -57,9 +57,6 @@
     <t>936.940.973.992.997.10163.20113.20159.20166.20173.20180.20200.20258.20272.20275.20290.20291.20331.40137.40143.50444.50607.50622.50819.50821.50825.60165.60190.60195.60202.60205.60206.60215.61004.70102.70638.90668</t>
   </si>
   <si>
-    <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425</t>
-  </si>
-  <si>
     <t>233.10167.20234.20292.20357.20379.20385.50102.50818.60124.60139.60158.60174.60258.70101.3.70114.20129</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163.50815.50808</t>
+  </si>
+  <si>
+    <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425.60126</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1:B994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -383,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -407,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -415,7 +415,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -423,7 +423,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -439,7 +439,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subi todas las imagenes de cod evo
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -69,13 +69,13 @@
     <t>12.20.265.938.947.970.999.1000.20094.20095.20108.20117.20140.20142.20156.20160.20169.20179.20242.20244.20249.20294.20344.20362.20364.20366.70106</t>
   </si>
   <si>
-    <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201.60270.60134</t>
-  </si>
-  <si>
     <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163.50815.50808</t>
   </si>
   <si>
     <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425.60126.40139</t>
+  </si>
+  <si>
+    <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201.60270.60134.40125</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1:B994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -415,7 +415,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -439,7 +439,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizar grupos de clientes
</commit_message>
<xml_diff>
--- a/excel/GRUPOS_CLIENTES.xlsx
+++ b/excel/GRUPOS_CLIENTES.xlsx
@@ -63,19 +63,19 @@
     <t>939.961.962.987.1002.1010.1012.10137.10158.10162.20106.20114.20118.20137.20174.20211.20224.20230.20257.20277.20281.20289.20296.20299.20301.20306.20319.20367.20371.20372.20374.20381.20386.20388.20391.20395.50224.50812.50813.50824.50827.60128.60130.60133.60148.60163.60196.60198.60222.60257.90621.40144</t>
   </si>
   <si>
-    <t>11.20096.20228.20238.20256.20260.20303.20361.40124.50805.60125.60191.60217.60253.61012.90504.90602.90671.90509</t>
-  </si>
-  <si>
     <t>33.237.251.308.946.950.952.958.963.965.969.10165.20101.20110.20128.20148.20164.20236.20241.20246.20271.20284.20293.20309.20351.20380.20163.50815.50808</t>
   </si>
   <si>
-    <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425.60126.40139</t>
-  </si>
-  <si>
     <t>5.27.246.920.951.954.956.972.974.980.982.989.994.1005.1007.10107.10157.10160.20109.20116.20120.20121.20146.20165.20178.20201.60270.60134.40125</t>
   </si>
   <si>
     <t>12.20.265.938.947.970.999.1000.20094.20095.20108.20117.20140.20142.20156.20160.20169.20179.20242.20244.20249.20294.20344.20362.20364.20366.70106.60109</t>
+  </si>
+  <si>
+    <t>11.20096.20228.20238.20256.20260.20303.20361.40124.50805.60125.60191.60217.60253.61012.90504.90602.90671.90509.20282</t>
+  </si>
+  <si>
+    <t>955.993.998.1001.1006.1009.10424.20103.20125.20310.20384.40151.50623.60159.60162.60192.60225.70103.70113.10425.60126.40139.20205</t>
   </si>
 </sst>
 </file>
@@ -358,8 +358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -407,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -415,7 +415,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -439,7 +439,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>